<commit_message>
Added house district data to precinct csv.
</commit_message>
<xml_diff>
--- a/precincts_2020_cleaned/district_to_precinct_merge/HsD2011_Intersect.xlsx
+++ b/precincts_2020_cleaned/district_to_precinct_merge/HsD2011_Intersect.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\avagnoz\Desktop\Clemson_Redistricting_Team\precincts_2020_cleaned\district_to_precinct_merge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{059535E8-509A-45A5-B20C-BE69D22190E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F76E3A13-3EEF-4124-90C0-837EE66929F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420"/>
+    <workbookView xWindow="1820" yWindow="1820" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HsD2011_Intersect" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" calcOnSave="0"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -403,7 +403,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -790,7 +790,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -798,7 +798,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:IV65536"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -18920,8 +18920,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B4615">
-    <sortCondition ref="A1:A4615"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B2264">
+    <sortCondition ref="A1:A2264"/>
   </sortState>
   <conditionalFormatting sqref="A1:A1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="1" stopIfTrue="1"/>

</xml_diff>